<commit_message>
Mery Moo sy nikal gae
</commit_message>
<xml_diff>
--- a/User Data/MARCH_2021/Monthly Report LHR 01-03-2021.xlsx
+++ b/User Data/MARCH_2021/Monthly Report LHR 01-03-2021.xlsx
@@ -1895,7 +1895,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H43"/>
+  <dimension ref="A2:H43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2332,20 +2332,6 @@
       <c r="G28" s="10" t="n"/>
       <c r="H28" s="10" t="n"/>
     </row>
-    <row r="29"/>
-    <row r="30"/>
-    <row r="31"/>
-    <row r="32"/>
-    <row r="33"/>
-    <row r="34"/>
-    <row r="35"/>
-    <row r="36"/>
-    <row r="37"/>
-    <row r="38"/>
-    <row r="39"/>
-    <row r="40"/>
-    <row r="41"/>
-    <row r="42"/>
     <row r="43">
       <c r="H43" t="inlineStr">
         <is>
@@ -2945,7 +2931,7 @@
     <row r="7" ht="15.75" customHeight="1" s="56">
       <c r="A7" s="30" t="inlineStr">
         <is>
-          <t>18/Mar/2021</t>
+          <t>24/Mar/2021</t>
         </is>
       </c>
       <c r="B7" s="30" t="n"/>
@@ -3891,7 +3877,7 @@
     <row r="7" ht="15.75" customHeight="1" s="56">
       <c r="A7" s="30" t="inlineStr">
         <is>
-          <t>18/Mar/2021</t>
+          <t>25/Mar/2021</t>
         </is>
       </c>
       <c r="B7" s="30" t="n"/>
@@ -4851,7 +4837,7 @@
     <row r="7" ht="15.75" customHeight="1" s="56">
       <c r="A7" s="30" t="inlineStr">
         <is>
-          <t>18/Mar/2021</t>
+          <t>30/Mar/2021</t>
         </is>
       </c>
       <c r="B7" s="30" t="n"/>

</xml_diff>